<commit_message>
Updated SOBP code with new baseline data
</commit_message>
<xml_diff>
--- a/TMS_CTRL_Demographics.xlsx
+++ b/TMS_CTRL_Demographics.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micaelawiseman/PhD/Thesis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwiseman\Desktop\Micaela rTMS Project\Winterlight_GH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E24D1EBD-8EB2-424B-9838-0132ED550CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" xr2:uid="{F532F060-933D-4B9E-ABBC-1E962AF898E5}"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="15000" windowHeight="18900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TMS" sheetId="1" r:id="rId1"/>
     <sheet name="CTRL" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="265">
   <si>
     <t>CTC001</t>
   </si>
@@ -727,12 +726,117 @@
   </si>
   <si>
     <t>OCD133</t>
+  </si>
+  <si>
+    <t>TMS054</t>
+  </si>
+  <si>
+    <t>TMS055</t>
+  </si>
+  <si>
+    <t>TMS056</t>
+  </si>
+  <si>
+    <t>TMS057</t>
+  </si>
+  <si>
+    <t>TMS058</t>
+  </si>
+  <si>
+    <t>TMS059</t>
+  </si>
+  <si>
+    <t>MFB13</t>
+  </si>
+  <si>
+    <t>MFB14</t>
+  </si>
+  <si>
+    <t>Dari</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>CTC060</t>
+  </si>
+  <si>
+    <t>CTC061</t>
+  </si>
+  <si>
+    <t>CTC062</t>
+  </si>
+  <si>
+    <t>CTC063</t>
+  </si>
+  <si>
+    <t>CTC064</t>
+  </si>
+  <si>
+    <t>CTC065</t>
+  </si>
+  <si>
+    <t>CTC066</t>
+  </si>
+  <si>
+    <t>CTC067</t>
+  </si>
+  <si>
+    <t>CTC068</t>
+  </si>
+  <si>
+    <t>CTC069</t>
+  </si>
+  <si>
+    <t>CTC070</t>
+  </si>
+  <si>
+    <t>CTC071</t>
+  </si>
+  <si>
+    <t>CTC072</t>
+  </si>
+  <si>
+    <t>CTC073</t>
+  </si>
+  <si>
+    <t>Punjabi</t>
+  </si>
+  <si>
+    <t>CTC074</t>
+  </si>
+  <si>
+    <t>CTC075</t>
+  </si>
+  <si>
+    <t>CTC076</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>CTC077</t>
+  </si>
+  <si>
+    <t>CTC078</t>
+  </si>
+  <si>
+    <t>CTC079</t>
+  </si>
+  <si>
+    <t>CTC080</t>
+  </si>
+  <si>
+    <t>CTC081</t>
+  </si>
+  <si>
+    <t>Konkani</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -860,7 +964,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Dark Mode" xfId="1" xr:uid="{7D5E7954-321F-44F7-B7B4-107633D73482}"/>
+    <cellStyle name="Dark Mode" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -1234,16 +1338,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3CAA2A-5D67-4DD0-B63B-DED191CBD016}">
-  <dimension ref="A1:AE66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1338,7 +1443,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1428,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1518,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1608,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1698,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1786,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1879,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1972,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2012,7 +2117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2102,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2192,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2282,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2372,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2460,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2550,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2638,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -2712,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2802,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2895,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2985,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -3075,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -3163,7 +3268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -3256,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -3346,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -3436,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>216</v>
       </c>
@@ -3456,7 +3561,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -3546,7 +3651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3588,7 +3693,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -3678,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -3720,7 +3825,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -3810,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -3900,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -3939,7 +4044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -4026,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -4113,7 +4218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -4203,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -4245,7 +4350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -4287,7 +4392,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -4329,7 +4434,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -4371,7 +4476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -4391,7 +4496,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -4429,7 +4534,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>104</v>
       </c>
@@ -4449,7 +4554,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>195</v>
       </c>
@@ -4487,7 +4592,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>196</v>
       </c>
@@ -4525,7 +4630,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>197</v>
       </c>
@@ -4563,7 +4668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>198</v>
       </c>
@@ -4601,7 +4706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>199</v>
       </c>
@@ -4639,7 +4744,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>200</v>
       </c>
@@ -4677,7 +4782,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>206</v>
       </c>
@@ -4715,7 +4820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>208</v>
       </c>
@@ -4753,7 +4858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>214</v>
       </c>
@@ -4773,7 +4878,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>215</v>
       </c>
@@ -4793,32 +4898,65 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>217</v>
       </c>
+      <c r="B54">
+        <v>1992</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>29</v>
+      </c>
       <c r="E54" t="s">
         <v>75</v>
       </c>
       <c r="F54" t="s">
         <v>67</v>
       </c>
+      <c r="G54">
+        <v>16</v>
+      </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>218</v>
       </c>
+      <c r="B55">
+        <v>1953</v>
+      </c>
+      <c r="C55">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>68</v>
+      </c>
       <c r="E55" t="s">
         <v>75</v>
       </c>
       <c r="F55" t="s">
         <v>67</v>
       </c>
+      <c r="G55">
+        <v>14</v>
+      </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>219</v>
       </c>
+      <c r="B56">
+        <v>1958</v>
+      </c>
+      <c r="C56">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>63</v>
+      </c>
       <c r="E56" t="s">
         <v>75</v>
       </c>
@@ -4826,7 +4964,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>220</v>
       </c>
@@ -4837,7 +4975,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>221</v>
       </c>
@@ -4848,7 +4986,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>222</v>
       </c>
@@ -4859,7 +4997,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>223</v>
       </c>
@@ -4870,7 +5008,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>224</v>
       </c>
@@ -4881,7 +5019,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>225</v>
       </c>
@@ -4892,7 +5030,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>226</v>
       </c>
@@ -4903,7 +5041,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>227</v>
       </c>
@@ -4914,7 +5052,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>228</v>
       </c>
@@ -4925,7 +5063,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4934,6 +5072,259 @@
       </c>
       <c r="F66" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>230</v>
+      </c>
+      <c r="B67">
+        <v>1997</v>
+      </c>
+      <c r="C67">
+        <v>11</v>
+      </c>
+      <c r="D67">
+        <v>26</v>
+      </c>
+      <c r="E67" t="s">
+        <v>76</v>
+      </c>
+      <c r="F67" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67">
+        <v>12</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67" t="s">
+        <v>210</v>
+      </c>
+      <c r="L67">
+        <v>4</v>
+      </c>
+      <c r="M67">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>231</v>
+      </c>
+      <c r="B68">
+        <v>1951</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>72</v>
+      </c>
+      <c r="E68" t="s">
+        <v>75</v>
+      </c>
+      <c r="F68" t="s">
+        <v>67</v>
+      </c>
+      <c r="G68">
+        <v>18</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
+        <v>59</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69">
+        <v>1955</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>68</v>
+      </c>
+      <c r="E69" t="s">
+        <v>76</v>
+      </c>
+      <c r="F69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G69">
+        <v>20</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69" t="s">
+        <v>59</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>233</v>
+      </c>
+      <c r="B70">
+        <v>1955</v>
+      </c>
+      <c r="C70">
+        <v>11</v>
+      </c>
+      <c r="D70">
+        <v>68</v>
+      </c>
+      <c r="E70" t="s">
+        <v>75</v>
+      </c>
+      <c r="F70" t="s">
+        <v>67</v>
+      </c>
+      <c r="G70">
+        <v>16</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>59</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>234</v>
+      </c>
+      <c r="B71">
+        <v>1951</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>73</v>
+      </c>
+      <c r="E71" t="s">
+        <v>76</v>
+      </c>
+      <c r="F71" t="s">
+        <v>68</v>
+      </c>
+      <c r="G71">
+        <v>18</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71" t="s">
+        <v>59</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>235</v>
+      </c>
+      <c r="B72">
+        <v>1987</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>37</v>
+      </c>
+      <c r="E72" t="s">
+        <v>76</v>
+      </c>
+      <c r="F72" t="s">
+        <v>68</v>
+      </c>
+      <c r="G72">
+        <v>16</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72" t="s">
+        <v>238</v>
+      </c>
+      <c r="L72">
+        <v>15</v>
+      </c>
+      <c r="M72">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>236</v>
+      </c>
+      <c r="B73">
+        <v>1983</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>40</v>
+      </c>
+      <c r="E73" t="s">
+        <v>75</v>
+      </c>
+      <c r="F73" t="s">
+        <v>67</v>
+      </c>
+      <c r="G73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -4944,20 +5335,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330999D-84C3-4399-84D6-744AA8A1E0B3}">
-  <dimension ref="A1:CO35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CO58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="22" max="24" width="8.83203125" customWidth="1"/>
+    <col min="22" max="24" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -5229,7 +5620,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5508,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5715,7 +6106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5994,7 +6385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -6273,7 +6664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -6549,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -6819,7 +7210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7026,7 +7417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -7302,7 +7693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -7572,7 +7963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -7851,7 +8242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -8121,7 +8512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -8400,7 +8791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -8673,7 +9064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -8952,7 +9343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -9084,7 +9475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -9363,7 +9754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>213</v>
       </c>
@@ -9633,7 +10024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -9903,7 +10294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -10104,7 +10495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -10311,7 +10702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -10512,7 +10903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -10685,7 +11076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -10964,7 +11355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -11243,7 +11634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -11300,7 +11691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -11435,7 +11826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -11638,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>211</v>
       </c>
@@ -11916,7 +12307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>209</v>
       </c>
@@ -12194,7 +12585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>190</v>
       </c>
@@ -12475,7 +12866,7 @@
       <c r="CN31" s="8"/>
       <c r="CO31" s="8"/>
     </row>
-    <row r="32" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>191</v>
       </c>
@@ -12609,7 +13000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>192</v>
       </c>
@@ -12887,7 +13278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>193</v>
       </c>
@@ -13093,7 +13484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>212</v>
       </c>
@@ -13131,7 +13522,7 @@
         <v>19</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35" si="14">MAX(S35:V35)+W35+MAX(X35:AA35)+AB35+AC35+AD35+AE35+AF35+MAX(AG35:AH35)</f>
+        <f t="shared" ref="M35:M36" si="14">MAX(S35:V35)+W35+MAX(X35:AA35)+AB35+AC35+AD35+AE35+AF35+MAX(AG35:AH35)</f>
         <v>7</v>
       </c>
       <c r="N35">
@@ -13371,9 +13762,577 @@
         <v>1</v>
       </c>
     </row>
+    <row r="36" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36">
+        <v>1958</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <f>2024-B36</f>
+        <v>66</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36">
+        <v>17</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>59</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f>D36-K36</f>
+        <v>62</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>2</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>1</v>
+      </c>
+      <c r="AG36">
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>240</v>
+      </c>
+      <c r="B37">
+        <v>1960</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:D53" si="20">2024-B37</f>
+        <v>64</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37">
+        <v>17</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>59</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>2</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>0</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37">
+        <v>0</v>
+      </c>
+      <c r="AG37">
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>241</v>
+      </c>
+      <c r="B38">
+        <v>1997</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="20"/>
+        <v>27</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38">
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>59</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <v>1</v>
+      </c>
+      <c r="AB38">
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>242</v>
+      </c>
+      <c r="B39">
+        <v>1996</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="20"/>
+        <v>28</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>67</v>
+      </c>
+      <c r="G39">
+        <v>16</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40">
+        <v>1987</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="20"/>
+        <v>37</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40">
+        <v>16</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42">
+        <v>1981</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="20"/>
+        <v>43</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42">
+        <v>20</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="45" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="46" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>249</v>
+      </c>
+      <c r="B46">
+        <v>1951</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="20"/>
+        <v>73</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46">
+        <v>18</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>250</v>
+      </c>
+      <c r="B47">
+        <v>1959</v>
+      </c>
+      <c r="D47">
+        <v>65</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47">
+        <v>18</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>253</v>
+      </c>
+      <c r="B50">
+        <v>1952</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="20"/>
+        <v>72</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50">
+        <v>16</v>
+      </c>
+      <c r="H50" t="s">
+        <v>239</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>255</v>
+      </c>
+      <c r="B51">
+        <v>1956</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="20"/>
+        <v>68</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>67</v>
+      </c>
+      <c r="G51">
+        <v>16</v>
+      </c>
+      <c r="H51" t="s">
+        <v>239</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>257</v>
+      </c>
+      <c r="B53">
+        <v>1960</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="20"/>
+        <v>64</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>67</v>
+      </c>
+      <c r="G53">
+        <v>16</v>
+      </c>
+      <c r="H53" t="s">
+        <v>239</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="M1:M1048576 O1:O1048576 Q1:Q1048576 S32:S35 U32:U35">
+  <conditionalFormatting sqref="S32:S35 U32:U35 M1:M35 M54:M1048576 L36:L53 O1:O35 O54:O1048576 N36:N53 Q1:Q35 Q54:Q1048576 P36:P53">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>11</formula>
       <formula>15</formula>
@@ -13383,12 +14342,12 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M1048576 O2:O1048576 Q2:Q1048576 S32:S35 U32:U35">
+  <conditionalFormatting sqref="S32:S35 U32:U35 M2:M35 M54:M1048576 L36:L53 O2:O35 O54:O1048576 N36:N53 Q2:Q35 Q54:Q1048576 P36:P53">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576 P1:P1048576 R1:R1048576 V32:AP34 T32:T35 AQ33:CL33 AQ34:BN34 V35:CL35">
+  <conditionalFormatting sqref="V32:AP34 T32:T35 AQ33:CL33 AQ34:BN34 V35:CL35 N1:N35 N54:N1048576 M36:M53 P1:P35 P54:P1048576 O36:O53 R1:R35 R54:R1048576 Q36:Q53 AG36:AH36 AF37:AF38 AG38:AH38">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>10</formula>
       <formula>14</formula>
@@ -13398,7 +14357,7 @@
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N1048576 P2:P1048576 R2:R1048576 V32:AP34 T32:T35 AQ33:CL33 AQ34:BN34 V35:CL35">
+  <conditionalFormatting sqref="V32:AP34 T32:T35 AQ33:CL33 AQ34:BN34 V35:CL35 N2:N35 N54:N1048576 M36:M53 P2:P35 P54:P1048576 O36:O53 R2:R35 R54:R1048576 Q36:Q53 AG36:AH36 AF37:AF38 AG38:AH38">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
@@ -13409,40 +14368,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D219C2BA-438D-3041-8A14-4DEBE96CA4C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>207</v>

</xml_diff>